<commit_message>
feat: added affort and other revitions for cost and time estimations
</commit_message>
<xml_diff>
--- a/sprint 5/Estimacion de costos y tiempo.xlsx
+++ b/sprint 5/Estimacion de costos y tiempo.xlsx
@@ -1,16 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29116"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RJBar\Downloads\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAB27D8A-C46F-46C9-9560-79D730A25C24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{641BEDEA-65FD-4E0A-AC55-3D1E21D3628A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Costos y tiempo" sheetId="2" r:id="rId1"/>
@@ -36,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="115">
   <si>
     <t>Factor de Peso de Actores</t>
   </si>
@@ -305,6 +300,9 @@
     <t>Estimación de Esfuerzo (Horas-Hombre)</t>
   </si>
   <si>
+    <t>Esfuerzo total:</t>
+  </si>
+  <si>
     <t>Esfuerzo (E)</t>
   </si>
   <si>
@@ -314,6 +312,15 @@
     <t>Horas-Hombre (HH)</t>
   </si>
   <si>
+    <t>Tipo de Actividad</t>
+  </si>
+  <si>
+    <t>Porciento</t>
+  </si>
+  <si>
+    <t>E (H/H)</t>
+  </si>
+  <si>
     <t>TDES</t>
   </si>
   <si>
@@ -321,13 +328,106 @@
   </si>
   <si>
     <t xml:space="preserve">Horas </t>
+  </si>
+  <si>
+    <t>Análisis</t>
+  </si>
+  <si>
+    <t>Diseño</t>
+  </si>
+  <si>
+    <t>Implementación</t>
+  </si>
+  <si>
+    <t>Pruebas</t>
+  </si>
+  <si>
+    <t>Sobrecarga (Otras actividades)</t>
+  </si>
+  <si>
+    <t>Esfuerzo total</t>
+  </si>
+  <si>
+    <t>Estimación de Costo</t>
+  </si>
+  <si>
+    <t>Costo total</t>
+  </si>
+  <si>
+    <t>GTQ</t>
+  </si>
+  <si>
+    <r>
+      <t>Coeficienete de costos indirectos (</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>K</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+      </rPr>
+      <t>Tarifa horaria promedio (</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+      </rPr>
+      <t>THP</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+      </rPr>
+      <t>) GTQ</t>
+    </r>
+  </si>
+  <si>
+    <t>1. 30 Quetzales la hora por persona (todos ganamos lo mismo)</t>
+  </si>
+  <si>
+    <t>Quetzales</t>
+  </si>
+  <si>
+    <t>2. Somos 5 personas en el proyecto</t>
+  </si>
+  <si>
+    <t>La hora</t>
+  </si>
+  <si>
+    <t>Hosting, base de datos y servicios externos = Q.5,000</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -358,6 +458,13 @@
       <family val="2"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
       <b/>
       <u/>
       <sz val="14"/>
@@ -366,8 +473,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -376,12 +494,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -390,6 +514,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -438,33 +577,77 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thick">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thick">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -480,6 +663,58 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>666750</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1200150</xdr:colOff>
+      <xdr:row>76</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{67780015-FAE9-D9DC-E698-51C8AD98833A}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{D422BBCE-BB30-75C8-4F93-FACE8C447ADB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1276350" y="11182350"/>
+          <a:ext cx="4572000" cy="190500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -799,23 +1034,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF0A8B3D-DD73-4020-A5BE-3F39D1E3BDDE}">
-  <dimension ref="B2:K74"/>
+  <dimension ref="B2:L84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="G59" sqref="G59"/>
+    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="60.54296875" customWidth="1"/>
+    <col min="2" max="2" width="60.5703125" customWidth="1"/>
     <col min="3" max="3" width="56" customWidth="1"/>
-    <col min="4" max="4" width="12.26953125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.26953125" customWidth="1"/>
-    <col min="10" max="10" width="16.1796875" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.28515625" customWidth="1"/>
+    <col min="10" max="10" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="2" spans="2:11" ht="18.75">
       <c r="B2" s="11" t="s">
         <v>0</v>
       </c>
@@ -823,7 +1058,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:11">
       <c r="I3" s="7" t="s">
         <v>2</v>
       </c>
@@ -834,7 +1069,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:11">
       <c r="B4" t="s">
         <v>5</v>
       </c>
@@ -852,7 +1087,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:11">
       <c r="B5" t="s">
         <v>7</v>
       </c>
@@ -870,7 +1105,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:11">
       <c r="B6" t="s">
         <v>9</v>
       </c>
@@ -888,17 +1123,17 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:11">
       <c r="I7" t="s">
         <v>11</v>
       </c>
       <c r="J7" s="3"/>
-      <c r="K7" s="15">
+      <c r="K7" s="21">
         <f>SUM(K4:K6)</f>
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="2:11" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:11" ht="18.75">
       <c r="B9" s="11" t="s">
         <v>12</v>
       </c>
@@ -906,7 +1141,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:11">
       <c r="B11" s="5" t="s">
         <v>14</v>
       </c>
@@ -920,7 +1155,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:11">
       <c r="B12" s="3" t="s">
         <v>18</v>
       </c>
@@ -934,7 +1169,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:11">
       <c r="B13" s="3" t="s">
         <v>20</v>
       </c>
@@ -948,7 +1183,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:11">
       <c r="B14" s="3" t="s">
         <v>21</v>
       </c>
@@ -962,7 +1197,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:11">
       <c r="B15" s="3" t="s">
         <v>23</v>
       </c>
@@ -976,7 +1211,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:11">
       <c r="B16" s="3" t="s">
         <v>25</v>
       </c>
@@ -990,7 +1225,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:5">
       <c r="B17" s="3" t="s">
         <v>26</v>
       </c>
@@ -1004,7 +1239,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:5">
       <c r="B18" s="3" t="s">
         <v>27</v>
       </c>
@@ -1018,7 +1253,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:5">
       <c r="B19" s="4" t="s">
         <v>28</v>
       </c>
@@ -1028,12 +1263,12 @@
       <c r="D19" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E19" s="19">
+      <c r="E19" s="26">
         <f>SUM(E12:E18)</f>
         <v>70</v>
       </c>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:5">
       <c r="B22" s="3" t="s">
         <v>1</v>
       </c>
@@ -1042,7 +1277,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:5">
       <c r="B23" s="8" t="s">
         <v>13</v>
       </c>
@@ -1051,16 +1286,16 @@
         <v>70</v>
       </c>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:5">
       <c r="B24" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C24" s="18">
+      <c r="C24" s="25">
         <f>C23+C22</f>
         <v>84</v>
       </c>
     </row>
-    <row r="27" spans="2:5" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="27" spans="2:5" ht="18.75">
       <c r="B27" s="9" t="s">
         <v>31</v>
       </c>
@@ -1069,12 +1304,12 @@
       </c>
       <c r="D27" s="10"/>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:5">
       <c r="B28" s="10"/>
       <c r="C28" s="10"/>
       <c r="D28" s="10"/>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:5">
       <c r="B29" s="10" t="s">
         <v>33</v>
       </c>
@@ -1083,12 +1318,12 @@
       </c>
       <c r="D29" s="10"/>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:5">
       <c r="B30" s="10"/>
       <c r="C30" s="10"/>
       <c r="D30" s="10"/>
     </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:5">
       <c r="B31" s="13" t="s">
         <v>35</v>
       </c>
@@ -1102,7 +1337,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:5">
       <c r="B32" s="12" t="s">
         <v>39</v>
       </c>
@@ -1116,7 +1351,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:5">
       <c r="B33" s="12" t="s">
         <v>41</v>
       </c>
@@ -1130,7 +1365,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:5">
       <c r="B34" s="12" t="s">
         <v>43</v>
       </c>
@@ -1144,7 +1379,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:5">
       <c r="B35" s="12" t="s">
         <v>45</v>
       </c>
@@ -1158,7 +1393,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:5">
       <c r="B36" s="12" t="s">
         <v>47</v>
       </c>
@@ -1172,7 +1407,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:5">
       <c r="B37" s="12" t="s">
         <v>49</v>
       </c>
@@ -1186,7 +1421,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:5">
       <c r="B38" s="12" t="s">
         <v>52</v>
       </c>
@@ -1200,7 +1435,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:5">
       <c r="B39" s="12" t="s">
         <v>54</v>
       </c>
@@ -1214,7 +1449,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:5">
       <c r="B40" s="12" t="s">
         <v>56</v>
       </c>
@@ -1228,7 +1463,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:5">
       <c r="B41" s="12" t="s">
         <v>58</v>
       </c>
@@ -1242,7 +1477,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:5">
       <c r="B42" s="12" t="s">
         <v>60</v>
       </c>
@@ -1256,7 +1491,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:5">
       <c r="B43" s="12" t="s">
         <v>62</v>
       </c>
@@ -1270,7 +1505,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:5">
       <c r="B44" s="13" t="s">
         <v>64</v>
       </c>
@@ -1284,36 +1519,36 @@
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:5">
       <c r="C45" t="s">
         <v>66</v>
       </c>
-      <c r="D45" s="16">
+      <c r="D45" s="22">
         <f>SUM(D32:D44)</f>
         <v>13</v>
       </c>
-      <c r="E45" s="15">
+      <c r="E45" s="21">
         <f>SUM(E32:E44)</f>
         <v>50</v>
       </c>
     </row>
-    <row r="46" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:5">
       <c r="D46" s="10"/>
     </row>
-    <row r="47" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="47" spans="2:5">
       <c r="B47" t="s">
         <v>34</v>
       </c>
-      <c r="C47" s="17">
+      <c r="C47" s="24">
         <f xml:space="preserve"> 0.6 + 0.01 * (D45*E45)</f>
         <v>7.1</v>
       </c>
       <c r="D47" s="10"/>
     </row>
-    <row r="48" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="48" spans="2:5">
       <c r="D48" s="10"/>
     </row>
-    <row r="49" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="49" spans="2:5">
       <c r="B49" s="10" t="s">
         <v>67</v>
       </c>
@@ -1322,12 +1557,12 @@
       </c>
       <c r="D49" s="10"/>
     </row>
-    <row r="50" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="50" spans="2:5">
       <c r="B50" s="10"/>
       <c r="C50" s="10"/>
       <c r="D50" s="10"/>
     </row>
-    <row r="51" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="51" spans="2:5">
       <c r="B51" s="13" t="s">
         <v>35</v>
       </c>
@@ -1341,7 +1576,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="52" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="52" spans="2:5">
       <c r="B52" s="12" t="s">
         <v>69</v>
       </c>
@@ -1355,7 +1590,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="53" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="53" spans="2:5">
       <c r="B53" s="12" t="s">
         <v>72</v>
       </c>
@@ -1369,7 +1604,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="54" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="54" spans="2:5">
       <c r="B54" s="12" t="s">
         <v>74</v>
       </c>
@@ -1383,7 +1618,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="55" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="55" spans="2:5">
       <c r="B55" s="12" t="s">
         <v>76</v>
       </c>
@@ -1397,7 +1632,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="56" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="56" spans="2:5">
       <c r="B56" s="12" t="s">
         <v>78</v>
       </c>
@@ -1411,7 +1646,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="57" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="57" spans="2:5">
       <c r="B57" s="12" t="s">
         <v>80</v>
       </c>
@@ -1425,7 +1660,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="58" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="58" spans="2:5">
       <c r="B58" s="12" t="s">
         <v>82</v>
       </c>
@@ -1439,7 +1674,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="59" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="59" spans="2:5">
       <c r="B59" s="13" t="s">
         <v>84</v>
       </c>
@@ -1453,23 +1688,23 @@
         <v>2</v>
       </c>
     </row>
-    <row r="60" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="60" spans="2:5">
       <c r="C60" t="s">
         <v>66</v>
       </c>
-      <c r="D60" s="16">
+      <c r="D60" s="22">
         <f>SUM(D52:D59)</f>
         <v>2</v>
       </c>
-      <c r="E60" s="15">
+      <c r="E60" s="21">
         <f>SUM(E52:E59)</f>
         <v>23</v>
       </c>
     </row>
-    <row r="61" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="61" spans="2:5">
       <c r="D61" s="10"/>
     </row>
-    <row r="62" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="62" spans="2:5">
       <c r="B62" t="s">
         <v>68</v>
       </c>
@@ -1479,17 +1714,17 @@
       </c>
       <c r="D62" s="10"/>
     </row>
-    <row r="63" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="63" spans="2:5">
       <c r="D63" s="10"/>
     </row>
-    <row r="64" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="64" spans="2:5">
       <c r="B64" s="10" t="s">
         <v>86</v>
       </c>
       <c r="C64" s="10"/>
       <c r="D64" s="10"/>
     </row>
-    <row r="65" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="65" spans="2:12">
       <c r="B65" s="10" t="s">
         <v>87</v>
       </c>
@@ -1499,70 +1734,218 @@
       </c>
       <c r="D65" s="10"/>
     </row>
-    <row r="66" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="66" spans="2:12">
       <c r="B66" s="10"/>
       <c r="C66" s="10"/>
       <c r="D66" s="10"/>
     </row>
-    <row r="67" spans="2:5" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="67" spans="2:12" ht="18.75">
       <c r="B67" s="9" t="s">
         <v>88</v>
       </c>
       <c r="C67" s="10"/>
       <c r="D67" s="10"/>
-    </row>
-    <row r="68" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="H67" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="68" spans="2:12">
       <c r="B68" s="10" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C68" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="D68" s="16">
+        <v>91</v>
+      </c>
+      <c r="D68" s="22">
         <f>C65*28</f>
         <v>333.98400000000026</v>
       </c>
       <c r="E68" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="69" spans="2:5" x14ac:dyDescent="0.35">
+        <v>92</v>
+      </c>
+      <c r="H68" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="I68" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="J68" s="15" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="69" spans="2:12">
       <c r="B69" s="10" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="C69" s="10" t="s">
-        <v>93</v>
+        <v>97</v>
+      </c>
+      <c r="D69" s="22">
+        <f>J74/5</f>
+        <v>166.99200000000013</v>
       </c>
       <c r="E69" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="70" spans="2:5" x14ac:dyDescent="0.35">
+        <v>98</v>
+      </c>
+      <c r="H69" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="I69" s="16">
+        <v>0.1</v>
+      </c>
+      <c r="J69" s="15">
+        <f>J70/2</f>
+        <v>83.496000000000066</v>
+      </c>
+    </row>
+    <row r="70" spans="2:12">
       <c r="B70" s="10"/>
       <c r="C70" s="10"/>
       <c r="D70" s="10"/>
-    </row>
-    <row r="71" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="H70" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="I70" s="16">
+        <v>0.2</v>
+      </c>
+      <c r="J70" s="15">
+        <f>J71/2</f>
+        <v>166.99200000000013</v>
+      </c>
+      <c r="L70">
+        <f>J71/0.4</f>
+        <v>834.9600000000006</v>
+      </c>
+    </row>
+    <row r="71" spans="2:12">
       <c r="B71" s="10"/>
       <c r="C71" s="10"/>
       <c r="D71" s="10"/>
-    </row>
-    <row r="72" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="H71" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="I71" s="16">
+        <v>0.4</v>
+      </c>
+      <c r="J71" s="15">
+        <f>D68</f>
+        <v>333.98400000000026</v>
+      </c>
+    </row>
+    <row r="72" spans="2:12">
       <c r="B72" s="10"/>
       <c r="C72" s="10"/>
       <c r="D72" s="10"/>
-    </row>
-    <row r="73" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="H72" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="I72" s="16">
+        <v>0.15</v>
+      </c>
+      <c r="J72" s="15">
+        <f>L70*I72</f>
+        <v>125.24400000000009</v>
+      </c>
+    </row>
+    <row r="73" spans="2:12">
       <c r="B73" s="10"/>
       <c r="C73" s="10"/>
       <c r="D73" s="10"/>
-    </row>
-    <row r="74" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="H73" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="I73" s="16">
+        <v>0.15</v>
+      </c>
+      <c r="J73" s="15">
+        <f>L70*I73</f>
+        <v>125.24400000000009</v>
+      </c>
+    </row>
+    <row r="74" spans="2:12">
       <c r="B74" s="10"/>
       <c r="C74" s="10"/>
       <c r="D74" s="10"/>
+      <c r="J74" s="21">
+        <f>SUM(J69:J73)</f>
+        <v>834.96000000000072</v>
+      </c>
+      <c r="K74" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="75" spans="2:12" ht="18.75">
+      <c r="B75" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="C75" s="10"/>
+      <c r="D75" s="10"/>
+    </row>
+    <row r="76" spans="2:12">
+      <c r="B76" s="10"/>
+      <c r="C76" s="10"/>
+    </row>
+    <row r="77" spans="2:12">
+      <c r="B77" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="C77" s="10"/>
+      <c r="D77" s="20">
+        <f>J74*C78*150</f>
+        <v>250488.0000000002</v>
+      </c>
+      <c r="E77" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="78" spans="2:12">
+      <c r="B78" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="C78" s="23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="79" spans="2:12">
+      <c r="B79" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="C79" s="18"/>
+    </row>
+    <row r="80" spans="2:12">
+      <c r="B80" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="C80" s="27">
+        <f>30*5</f>
+        <v>150</v>
+      </c>
+      <c r="D80" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="81" spans="2:4">
+      <c r="B81" s="17" t="s">
+        <v>112</v>
+      </c>
+      <c r="C81" s="27"/>
+      <c r="D81" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="84" spans="2:4">
+      <c r="B84" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="C84" s="18">
+        <v>5060</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C80:C81"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>